<commit_message>
fixed general danger signs
changed ! to selected('no')
</commit_message>
<xml_diff>
--- a/form-files/adaptiveIMCI_clinician/clinician.xlsx
+++ b/form-files/adaptiveIMCI_clinician/clinician.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9570"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="9570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="728" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="514">
   <si>
     <t>type</t>
   </si>
@@ -1508,9 +1508,6 @@
     <t>calculates.high_danger_pneumonia() == "danger" ? "Danger" : calculates.med_danger_pneumonia() == "danger" ? "Present" : "Not present"</t>
   </si>
   <si>
-    <t>!calculates.can_drink() || calculates.is_vomiting() ||calculates.has_convulsions() ? "Danger" : "Not present"</t>
-  </si>
-  <si>
     <t>calculates.general_danger_level() == "Danger" || calculates.high_danger_malaria() == "danger" || calculates.high_danger_pneumonia() == "danger" || calculates.high_danger_diarrhea() == "danger" || calculates.high_danger_malaria() == "danger"|| calculates.high_danger_measles() == "danger" || calculates.high_danger_ear() == "danger" || calculates.high_danger_malnut() == "danger" || calculates.high_danger_anemia() == "danger" ? "danger" : "good"</t>
   </si>
   <si>
@@ -1554,6 +1551,15 @@
   </si>
   <si>
     <t>{{calculates.med_danger_anemia() == "danger" &amp;&amp; !(calculates.low_danger_pneumonia() == "danger" || calculates.med_danger_dehydration() == "danger" || calculates.med_danger_ear() == "danger" || calculates.low_danger_dehydration() == "danger" || calculates.med_danger_diarrhea() == "danger" || calculates.severe_classification() == "danger" || calculates.high_danger_diarrhea() == "danger"|| calculates.med_danger_pneumonia() == "danger" || calculates.danger_dysentry()== "danger" || calculates.med_danger_measles() == "danger"  || calculates.med_danger_malaria() == "danger" || calculates.low_danger_malaria() == "danger") ? "danger" : "good"}}</t>
+  </si>
+  <si>
+    <t>cannot_drink</t>
+  </si>
+  <si>
+    <t>selected(data('drink'),'no')</t>
+  </si>
+  <si>
+    <t>calculates.cannot_drink() || calculates.is_vomiting() ||calculates.has_convulsions() ? "Danger" : "Not present"</t>
   </si>
 </sst>
 </file>
@@ -1985,7 +1991,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1995,7 +2001,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S85"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
@@ -2805,7 +2811,7 @@
       <c r="Q29" s="4"/>
       <c r="R29" s="4"/>
     </row>
-    <row r="30" spans="1:18" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
         <v>24</v>
       </c>
@@ -4054,9 +4060,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD111"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B109" sqref="B109"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B81" sqref="B81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4105,6 +4111,14 @@
       </c>
       <c r="B6" s="1" t="s">
         <v>69</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -53546,7 +53560,7 @@
         <v>437</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -53554,7 +53568,7 @@
         <v>92</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>496</v>
+        <v>513</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -53935,6 +53949,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -54236,7 +54251,7 @@
         <v>422</v>
       </c>
       <c r="J14" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -54247,7 +54262,7 @@
         <v>417</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>422</v>
@@ -54270,7 +54285,7 @@
         <v>422</v>
       </c>
       <c r="J16" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -54384,7 +54399,7 @@
         <v>235</v>
       </c>
       <c r="J24" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -54632,14 +54647,14 @@
         <v>230</v>
       </c>
       <c r="B43" s="5" t="s">
+        <v>501</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>502</v>
-      </c>
-      <c r="C43" s="5" t="s">
-        <v>503</v>
       </c>
       <c r="E43" s="5"/>
       <c r="J43" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
@@ -54673,7 +54688,7 @@
         <v>245</v>
       </c>
       <c r="J46" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
@@ -54754,7 +54769,7 @@
       </c>
       <c r="E52" s="5"/>
       <c r="J52" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
@@ -54811,7 +54826,7 @@
         <v>415</v>
       </c>
       <c r="J56" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.25">
@@ -54855,7 +54870,7 @@
         <v>250</v>
       </c>
       <c r="J61" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
@@ -54884,7 +54899,7 @@
       </c>
       <c r="E63" s="5"/>
       <c r="J63" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.25">
@@ -55034,7 +55049,7 @@
       </c>
       <c r="E77" s="5"/>
       <c r="J77" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.25">
@@ -55094,7 +55109,7 @@
       </c>
       <c r="E82" s="5"/>
       <c r="J82" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
experimental: jump directly to menu
</commit_message>
<xml_diff>
--- a/form-files/adaptiveIMCI_clinician/clinician.xlsx
+++ b/form-files/adaptiveIMCI_clinician/clinician.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="754" uniqueCount="531">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="534">
   <si>
     <t>type</t>
   </si>
@@ -1617,6 +1617,15 @@
   <si>
     <t>data('fever_days') &gt; 0</t>
   </si>
+  <si>
+    <t>label menu</t>
+  </si>
+  <si>
+    <t>goto menu</t>
+  </si>
+  <si>
+    <t>get_patient_name != null</t>
+  </si>
 </sst>
 </file>
 
@@ -1764,7 +1773,7 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1"/>
@@ -1803,6 +1812,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Bad" xfId="5" builtinId="27"/>
@@ -2089,11 +2099,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S95"/>
+  <dimension ref="A1:S97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I56" sqref="I56"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2175,65 +2185,49 @@
         <v>220</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>129</v>
-      </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="13"/>
-      <c r="K2" s="13"/>
-      <c r="L2" s="13"/>
-      <c r="M2" s="13"/>
-      <c r="N2" s="13"/>
-      <c r="O2" s="13"/>
-      <c r="P2" s="13"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
+    <row r="2" spans="1:19" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="21" t="s">
+        <v>532</v>
+      </c>
+      <c r="C2" t="s">
+        <v>533</v>
+      </c>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
+      <c r="A3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B3" s="13"/>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A4" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="F4" s="14"/>
+      <c r="A4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
@@ -2248,27 +2242,24 @@
       <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>141</v>
+      <c r="A5" s="13" t="s">
+        <v>23</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F5" s="4"/>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="14"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
-      <c r="J5" s="1" t="s">
-        <v>524</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="L5" s="13"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
@@ -2280,19 +2271,19 @@
       <c r="A6" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B6" s="13"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>125</v>
+        <v>41</v>
       </c>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="J6" s="1" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>527</v>
@@ -2306,26 +2297,27 @@
       <c r="R6" s="4"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="4"/>
+      <c r="A7" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B7" s="13"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>138</v>
-      </c>
+        <v>125</v>
+      </c>
+      <c r="F7" s="4"/>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
+      <c r="J7" s="1" t="s">
+        <v>525</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>527</v>
+      </c>
+      <c r="L7" s="13"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
@@ -2335,13 +2327,19 @@
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
@@ -2356,8 +2354,8 @@
       <c r="R8" s="4"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="20" t="s">
-        <v>494</v>
+      <c r="A9" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2378,8 +2376,8 @@
       <c r="R9" s="4"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>139</v>
+      <c r="A10" s="20" t="s">
+        <v>494</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2400,12 +2398,10 @@
       <c r="R10" s="4"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>128</v>
-      </c>
+      <c r="A11" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -2424,20 +2420,16 @@
       <c r="R11" s="4"/>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="4"/>
+      <c r="A12" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>128</v>
+      </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -2458,10 +2450,10 @@
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>138</v>
@@ -2486,10 +2478,10 @@
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F14" s="4" t="s">
         <v>138</v>
@@ -2509,13 +2501,19 @@
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -2530,12 +2528,10 @@
       <c r="R15" s="4"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>36</v>
-      </c>
+      <c r="A16" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
@@ -2554,19 +2550,16 @@
       <c r="R16" s="4"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>24</v>
+      <c r="A17" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -2584,13 +2577,12 @@
       <c r="A18" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4" t="s">
-        <v>55</v>
+        <v>124</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F18" s="4" t="s">
         <v>138</v>
@@ -2615,10 +2607,10 @@
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F19" s="4" t="s">
         <v>138</v>
@@ -2643,10 +2635,10 @@
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>34</v>
+        <v>57</v>
       </c>
       <c r="F20" s="4" t="s">
         <v>138</v>
@@ -2666,13 +2658,19 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
+      <c r="D21" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -2687,8 +2685,8 @@
       <c r="R21" s="4"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="20" t="s">
-        <v>495</v>
+      <c r="A22" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -2709,13 +2707,11 @@
       <c r="R22" s="4"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A23" s="21" t="s">
-        <v>496</v>
+      <c r="A23" s="20" t="s">
+        <v>495</v>
       </c>
       <c r="B23" s="4"/>
-      <c r="C23" s="22" t="s">
-        <v>497</v>
-      </c>
+      <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
@@ -2733,11 +2729,13 @@
       <c r="R23" s="4"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
-        <v>131</v>
+      <c r="A24" s="21" t="s">
+        <v>496</v>
       </c>
       <c r="B24" s="4"/>
-      <c r="C24" s="4"/>
+      <c r="C24" s="22" t="s">
+        <v>497</v>
+      </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
@@ -2754,60 +2752,50 @@
       <c r="Q24" s="4"/>
       <c r="R24" s="4"/>
     </row>
-    <row r="25" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="11" t="s">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="4"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="4"/>
+      <c r="O25" s="4"/>
+      <c r="P25" s="4"/>
+      <c r="Q25" s="4"/>
+      <c r="R25" s="4"/>
+    </row>
+    <row r="26" spans="1:18" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="D25" s="4"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="1" t="s">
-        <v>526</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="L26" s="4"/>
-      <c r="M26" s="4"/>
-      <c r="N26" s="4"/>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
-      <c r="Q26" s="4"/>
-      <c r="R26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11"/>
+      <c r="R26" s="11"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
@@ -2815,18 +2803,20 @@
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="15"/>
-      <c r="D27" s="4" t="s">
-        <v>142</v>
+      <c r="D27" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="F27" s="4"/>
+        <v>146</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="1" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>527</v>
@@ -2841,24 +2831,26 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="15"/>
-      <c r="D28" s="1" t="s">
-        <v>194</v>
+      <c r="D28" s="4" t="s">
+        <v>142</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>138</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="F28" s="4"/>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
-      <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
+      <c r="J28" s="1" t="s">
+        <v>528</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>527</v>
+      </c>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
@@ -2869,13 +2861,19 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="15"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
+      <c r="D29" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
@@ -2890,8 +2888,8 @@
       <c r="R29" s="4"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A30" s="20" t="s">
-        <v>498</v>
+      <c r="A30" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="15"/>
@@ -2912,13 +2910,11 @@
       <c r="R30" s="4"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A31" s="21" t="s">
-        <v>499</v>
+      <c r="A31" s="20" t="s">
+        <v>498</v>
       </c>
       <c r="B31" s="4"/>
-      <c r="C31" s="1" t="s">
-        <v>500</v>
-      </c>
+      <c r="C31" s="15"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
@@ -2936,10 +2932,13 @@
       <c r="R31" s="4"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
-        <v>145</v>
+      <c r="A32" s="21" t="s">
+        <v>499</v>
       </c>
       <c r="B32" s="4"/>
+      <c r="C32" s="1" t="s">
+        <v>500</v>
+      </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
@@ -2957,12 +2956,10 @@
       <c r="R32" s="4"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>162</v>
-      </c>
+      <c r="A33" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="B33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
@@ -2971,7 +2968,7 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
-      <c r="L33" s="13"/>
+      <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
@@ -2980,30 +2977,21 @@
       <c r="R33" s="4"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B34" s="4"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="A34" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
       <c r="I34" s="4"/>
-      <c r="J34" s="1" t="s">
-        <v>529</v>
-      </c>
-      <c r="K34" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="L34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="13"/>
       <c r="M34" s="4"/>
       <c r="N34" s="4"/>
       <c r="O34" s="4"/>
@@ -3013,15 +3001,15 @@
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="B35" s="4"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4" t="s">
-        <v>148</v>
+      <c r="C35" s="15"/>
+      <c r="D35" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="F35" s="4" t="s">
         <v>138</v>
@@ -3029,8 +3017,12 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
       <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
+      <c r="J35" s="1" t="s">
+        <v>529</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>527</v>
+      </c>
       <c r="L35" s="4"/>
       <c r="M35" s="4"/>
       <c r="N35" s="4"/>
@@ -3040,18 +3032,18 @@
       <c r="R35" s="4"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A36" s="1" t="s">
+      <c r="A36" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
-      <c r="D36" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>288</v>
-      </c>
-      <c r="F36" s="1" t="s">
+      <c r="D36" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F36" s="4" t="s">
         <v>138</v>
       </c>
       <c r="G36" s="4"/>
@@ -3074,10 +3066,10 @@
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="F37" s="1" t="s">
         <v>138</v>
@@ -3102,10 +3094,10 @@
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
       <c r="D38" s="1" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>138</v>
@@ -3130,10 +3122,10 @@
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="1" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="F39" s="1" t="s">
         <v>138</v>
@@ -3158,10 +3150,10 @@
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
       <c r="D40" s="1" t="s">
-        <v>293</v>
+        <v>304</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>294</v>
+        <v>305</v>
       </c>
       <c r="F40" s="1" t="s">
         <v>138</v>
@@ -3180,18 +3172,18 @@
       <c r="R40" s="4"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
-      <c r="D41" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="E41" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="F41" s="4" t="s">
+      <c r="D41" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="F41" s="1" t="s">
         <v>138</v>
       </c>
       <c r="G41" s="4"/>
@@ -3209,13 +3201,19 @@
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
+      <c r="D42" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="G42" s="4"/>
       <c r="H42" s="4"/>
       <c r="I42" s="4"/>
@@ -3230,8 +3228,8 @@
       <c r="R42" s="4"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A43" s="20" t="s">
-        <v>501</v>
+      <c r="A43" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -3252,13 +3250,11 @@
       <c r="R43" s="4"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A44" s="21" t="s">
-        <v>502</v>
+      <c r="A44" s="20" t="s">
+        <v>501</v>
       </c>
       <c r="B44" s="4"/>
-      <c r="C44" s="1" t="s">
-        <v>503</v>
-      </c>
+      <c r="C44" s="4"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
@@ -3276,10 +3272,13 @@
       <c r="R44" s="4"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="s">
-        <v>185</v>
+      <c r="A45" s="21" t="s">
+        <v>502</v>
       </c>
       <c r="B45" s="4"/>
+      <c r="C45" s="1" t="s">
+        <v>503</v>
+      </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
@@ -3297,12 +3296,10 @@
       <c r="R45" s="4"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A46" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>163</v>
-      </c>
+      <c r="A46" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B46" s="4"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
@@ -3311,7 +3308,7 @@
       <c r="I46" s="4"/>
       <c r="J46" s="4"/>
       <c r="K46" s="4"/>
-      <c r="L46" s="13"/>
+      <c r="L46" s="4"/>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
       <c r="O46" s="4"/>
@@ -3320,20 +3317,15 @@
       <c r="R46" s="4"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A47" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="1" t="s">
-        <v>248</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>247</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>138</v>
-      </c>
+      <c r="A47" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
       <c r="G47" s="4"/>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
@@ -3348,30 +3340,26 @@
       <c r="R47" s="4"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
-        <v>141</v>
+      <c r="A48" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B48" s="4"/>
-      <c r="C48" s="15"/>
+      <c r="C48" s="4"/>
       <c r="D48" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E48" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="F48" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="F48" s="1" t="s">
         <v>138</v>
       </c>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
-      <c r="J48" s="1" t="s">
-        <v>530</v>
-      </c>
-      <c r="K48" s="1" t="s">
-        <v>527</v>
-      </c>
-      <c r="L48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="13"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
@@ -3381,15 +3369,15 @@
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
-        <v>24</v>
+        <v>141</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="15"/>
-      <c r="D49" s="4" t="s">
-        <v>159</v>
+      <c r="D49" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>138</v>
@@ -3397,8 +3385,12 @@
       <c r="G49" s="4"/>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
+      <c r="J49" s="1" t="s">
+        <v>530</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>527</v>
+      </c>
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
@@ -3412,12 +3404,12 @@
         <v>24</v>
       </c>
       <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
+      <c r="C50" s="15"/>
       <c r="D50" s="4" t="s">
-        <v>153</v>
+        <v>159</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>138</v>
@@ -3442,10 +3434,10 @@
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
       <c r="D51" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>138</v>
@@ -3470,10 +3462,10 @@
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>138</v>
@@ -3493,13 +3485,19 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
+      <c r="D53" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F53" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
@@ -3514,15 +3512,11 @@
       <c r="R53" s="4"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A54" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>163</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>161</v>
-      </c>
+      <c r="A54" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B54" s="4"/>
+      <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
       <c r="F54" s="4"/>
@@ -3531,7 +3525,7 @@
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
-      <c r="L54" s="13"/>
+      <c r="L54" s="4"/>
       <c r="M54" s="4"/>
       <c r="N54" s="4"/>
       <c r="O54" s="4"/>
@@ -3540,26 +3534,24 @@
       <c r="R54" s="4"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="F55" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="A55" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="D55" s="4"/>
+      <c r="E55" s="4"/>
+      <c r="F55" s="4"/>
       <c r="G55" s="4"/>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="4"/>
-      <c r="L55" s="4"/>
+      <c r="L55" s="13"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
       <c r="O55" s="4"/>
@@ -3574,10 +3566,10 @@
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="E56" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>255</v>
       </c>
       <c r="F56" s="4" t="s">
         <v>138</v>
@@ -3602,10 +3594,10 @@
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F57" s="4" t="s">
         <v>138</v>
@@ -3625,13 +3617,19 @@
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
-      <c r="F58" s="4"/>
+      <c r="D58" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F58" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
@@ -3646,8 +3644,8 @@
       <c r="R58" s="4"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A59" s="20" t="s">
-        <v>504</v>
+      <c r="A59" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
@@ -3668,8 +3666,8 @@
       <c r="R59" s="4"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A60" s="2" t="s">
-        <v>132</v>
+      <c r="A60" s="20" t="s">
+        <v>504</v>
       </c>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
@@ -3690,12 +3688,11 @@
       <c r="R60" s="4"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A61" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>122</v>
-      </c>
+      <c r="A61" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B61" s="4"/>
+      <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
       <c r="F61" s="4"/>
@@ -3704,7 +3701,7 @@
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
       <c r="K61" s="4"/>
-      <c r="L61" s="13"/>
+      <c r="L61" s="4"/>
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
       <c r="O61" s="4"/>
@@ -3713,26 +3710,21 @@
       <c r="R61" s="4"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F62" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="A62" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4"/>
+      <c r="F62" s="4"/>
       <c r="G62" s="4"/>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
       <c r="J62" s="4"/>
       <c r="K62" s="4"/>
-      <c r="L62" s="4"/>
+      <c r="L62" s="13"/>
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
       <c r="O62" s="4"/>
@@ -3747,10 +3739,10 @@
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F63" s="4" t="s">
         <v>138</v>
@@ -3769,18 +3761,18 @@
       <c r="R63" s="4"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A64" s="1" t="s">
+      <c r="A64" s="4" t="s">
         <v>24</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
-      <c r="D64" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="E64" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="F64" s="1" t="s">
+      <c r="D64" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F64" s="4" t="s">
         <v>138</v>
       </c>
       <c r="G64" s="4"/>
@@ -3797,18 +3789,18 @@
       <c r="R64" s="4"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A65" s="4" t="s">
+      <c r="A65" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
-      <c r="D65" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F65" s="4" t="s">
+      <c r="D65" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>138</v>
       </c>
       <c r="G65" s="4"/>
@@ -3826,13 +3818,19 @@
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
-      <c r="F66" s="4"/>
+      <c r="D66" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>138</v>
+      </c>
       <c r="G66" s="4"/>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
@@ -3847,8 +3845,8 @@
       <c r="R66" s="4"/>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A67" s="20" t="s">
-        <v>505</v>
+      <c r="A67" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
@@ -3869,8 +3867,8 @@
       <c r="R67" s="4"/>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
-        <v>180</v>
+      <c r="A68" s="20" t="s">
+        <v>505</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="4"/>
@@ -3891,12 +3889,11 @@
       <c r="R68" s="4"/>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A69" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>169</v>
-      </c>
+      <c r="A69" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
       <c r="F69" s="4"/>
@@ -3905,7 +3902,7 @@
       <c r="I69" s="4"/>
       <c r="J69" s="4"/>
       <c r="K69" s="4"/>
-      <c r="L69" s="13"/>
+      <c r="L69" s="4"/>
       <c r="M69" s="4"/>
       <c r="N69" s="4"/>
       <c r="O69" s="4"/>
@@ -3914,26 +3911,21 @@
       <c r="R69" s="4"/>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A70" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="E70" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="F70" s="4" t="s">
-        <v>138</v>
-      </c>
+      <c r="A70" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4"/>
+      <c r="F70" s="4"/>
       <c r="G70" s="4"/>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
       <c r="J70" s="4"/>
       <c r="K70" s="4"/>
-      <c r="L70" s="4"/>
+      <c r="L70" s="13"/>
       <c r="M70" s="4"/>
       <c r="N70" s="4"/>
       <c r="O70" s="4"/>
@@ -3948,10 +3940,10 @@
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F71" s="4" t="s">
         <v>138</v>
@@ -3976,10 +3968,10 @@
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
       <c r="D72" s="4" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F72" s="4" t="s">
         <v>138</v>
@@ -4004,10 +3996,10 @@
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
       <c r="D73" s="4" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="F73" s="4" t="s">
         <v>138</v>
@@ -4026,20 +4018,18 @@
       <c r="R73" s="4"/>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+      <c r="A74" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B74" s="18" t="s">
-        <v>376</v>
-      </c>
-      <c r="C74" s="1"/>
-      <c r="D74" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="F74" s="1" t="s">
+      <c r="B74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F74" s="4" t="s">
         <v>138</v>
       </c>
       <c r="G74" s="4"/>
@@ -4056,14 +4046,22 @@
       <c r="R74" s="4"/>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A75" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
+      <c r="A75" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B75" s="18" t="s">
+        <v>376</v>
+      </c>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="G75" s="4"/>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
@@ -4078,8 +4076,8 @@
       <c r="R75" s="4"/>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A76" s="20" t="s">
-        <v>506</v>
+      <c r="A76" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -4100,22 +4098,16 @@
       <c r="R76" s="4"/>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A77" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B77" s="4" t="s">
-        <v>186</v>
-      </c>
+      <c r="A77" s="20" t="s">
+        <v>506</v>
+      </c>
+      <c r="B77" s="4"/>
       <c r="C77" s="4"/>
-      <c r="D77" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E77" s="14"/>
-      <c r="F77" s="14"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="4"/>
+      <c r="F77" s="4"/>
       <c r="G77" s="4"/>
-      <c r="H77" s="4" t="s">
-        <v>513</v>
-      </c>
+      <c r="H77" s="4"/>
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
       <c r="K77" s="4"/>
@@ -4128,16 +4120,12 @@
       <c r="R77" s="4"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A78" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>211</v>
-      </c>
+      <c r="A78" s="24" t="s">
+        <v>531</v>
+      </c>
+      <c r="B78" s="4"/>
       <c r="C78" s="4"/>
-      <c r="D78" s="1" t="s">
-        <v>507</v>
-      </c>
+      <c r="D78" s="4"/>
       <c r="E78" s="4"/>
       <c r="F78" s="4"/>
       <c r="G78" s="4"/>
@@ -4154,20 +4142,22 @@
       <c r="R78" s="4"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A79" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B79" s="4"/>
+      <c r="A79" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>186</v>
+      </c>
       <c r="C79" s="4"/>
-      <c r="D79" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="F79" s="4"/>
+      <c r="D79" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E79" s="14"/>
+      <c r="F79" s="14"/>
       <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
+      <c r="H79" s="4" t="s">
+        <v>513</v>
+      </c>
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
       <c r="K79" s="4"/>
@@ -4180,17 +4170,17 @@
       <c r="R79" s="4"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A80" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B80" s="4"/>
+      <c r="A80" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>211</v>
+      </c>
       <c r="C80" s="4"/>
       <c r="D80" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>216</v>
-      </c>
+        <v>507</v>
+      </c>
+      <c r="E80" s="4"/>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
       <c r="H80" s="4"/>
@@ -4207,14 +4197,16 @@
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="E81" s="1"/>
+        <v>213</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>214</v>
+      </c>
       <c r="F81" s="4"/>
       <c r="G81" s="4"/>
       <c r="H81" s="4"/>
@@ -4228,9 +4220,6 @@
       <c r="P81" s="4"/>
       <c r="Q81" s="4"/>
       <c r="R81" s="4"/>
-      <c r="S81" s="3" t="s">
-        <v>219</v>
-      </c>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
@@ -4239,10 +4228,10 @@
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
       <c r="D82" s="1" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F82" s="4"/>
       <c r="G82" s="4"/>
@@ -4260,12 +4249,12 @@
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="1" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="4"/>
@@ -4287,12 +4276,16 @@
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
-        <v>47</v>
+        <v>212</v>
       </c>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
-      <c r="D84" s="1"/>
-      <c r="E84" s="1"/>
+      <c r="D84" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>222</v>
+      </c>
       <c r="F84" s="4"/>
       <c r="G84" s="4"/>
       <c r="H84" s="4"/>
@@ -4308,19 +4301,56 @@
       <c r="R84" s="4"/>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A85" s="12"/>
+      <c r="A85" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="B85" s="4"/>
+      <c r="C85" s="4"/>
+      <c r="D85" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="E85" s="1"/>
+      <c r="F85" s="4"/>
+      <c r="G85" s="4"/>
+      <c r="H85" s="4"/>
+      <c r="I85" s="4"/>
+      <c r="J85" s="4"/>
+      <c r="K85" s="4"/>
+      <c r="L85" s="4"/>
+      <c r="M85" s="4"/>
+      <c r="N85" s="4"/>
+      <c r="O85" s="4"/>
+      <c r="P85" s="4"/>
+      <c r="Q85" s="4"/>
+      <c r="R85" s="4"/>
+      <c r="S85" s="3" t="s">
+        <v>219</v>
+      </c>
     </row>
-    <row r="92" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A92" s="16"/>
-      <c r="D92" s="16"/>
-      <c r="E92" s="17"/>
-      <c r="F92" s="17"/>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B86" s="4"/>
+      <c r="C86" s="4"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="4"/>
+      <c r="G86" s="4"/>
+      <c r="H86" s="4"/>
+      <c r="I86" s="4"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="4"/>
+      <c r="L86" s="4"/>
+      <c r="M86" s="4"/>
+      <c r="N86" s="4"/>
+      <c r="O86" s="4"/>
+      <c r="P86" s="4"/>
+      <c r="Q86" s="4"/>
+      <c r="R86" s="4"/>
     </row>
-    <row r="93" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A93" s="16"/>
-      <c r="D93" s="16"/>
-      <c r="E93" s="17"/>
-      <c r="F93" s="17"/>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A87" s="12"/>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A94" s="16"/>
@@ -4333,6 +4363,18 @@
       <c r="D95" s="16"/>
       <c r="E95" s="17"/>
       <c r="F95" s="17"/>
+    </row>
+    <row r="96" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A96" s="16"/>
+      <c r="D96" s="16"/>
+      <c r="E96" s="17"/>
+      <c r="F96" s="17"/>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97" s="16"/>
+      <c r="D97" s="16"/>
+      <c r="E97" s="17"/>
+      <c r="F97" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4374,8 +4416,8 @@
   <dimension ref="A1:XFD112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
jump directly to summary in clinician version if name has been entered
</commit_message>
<xml_diff>
--- a/form-files/adaptiveIMCI_clinician/clinician.xlsx
+++ b/form-files/adaptiveIMCI_clinician/clinician.xlsx
@@ -1624,7 +1624,7 @@
     <t>goto menu</t>
   </si>
   <si>
-    <t>get_patient_name != null</t>
+    <t>data('patient_name') != null</t>
   </si>
 </sst>
 </file>
@@ -2103,7 +2103,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4416,8 +4416,8 @@
   <dimension ref="A1:XFD112"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A29" sqref="A29"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
add version label to form version field
</commit_message>
<xml_diff>
--- a/form-files/adaptiveIMCI_clinician/clinician.xlsx
+++ b/form-files/adaptiveIMCI_clinician/clinician.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="120" windowWidth="20736" windowHeight="9456"/>
+    <workbookView xWindow="0" yWindow="120" windowWidth="20736" windowHeight="9456" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="534">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="535">
   <si>
     <t>type</t>
   </si>
@@ -1626,6 +1626,9 @@
   <si>
     <t>data('patient_name') != null</t>
   </si>
+  <si>
+    <t>0.9-clinician</t>
+  </si>
 </sst>
 </file>
 
@@ -2101,7 +2104,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
@@ -55360,9 +55363,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -55403,8 +55406,8 @@
       <c r="A4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="13">
-        <v>0.9</v>
+      <c r="B4" s="13" t="s">
+        <v>534</v>
       </c>
       <c r="C4" s="6"/>
     </row>

</xml_diff>